<commit_message>
criacao do excel para estudo de tabelas dinamicas e filtros
</commit_message>
<xml_diff>
--- a/Fundamentos/2 - Criação de Tabelas Dinâmicas/Base de Dados.xlsx
+++ b/Fundamentos/2 - Criação de Tabelas Dinâmicas/Base de Dados.xlsx
@@ -5,27 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicam\Desktop\Analista de Dados\Excel\estudos_excel\Fórmulas e Funções Avançadas\2 - Criação de Tabelas Dinâmicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicam\Desktop\Analista de Dados\Excel\estudos_excel\Fundamentos\2 - Criação de Tabelas Dinâmicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E546F3D-DA4F-4C93-9867-4F02DDF79D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75208A2-050B-42D9-80B8-C3723A1A9C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E8CAFAB-C6CE-4E40-90F1-1F95FAD07FF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Base de Dados" sheetId="33" r:id="rId1"/>
-    <sheet name="Formatação" sheetId="55" state="hidden" r:id="rId2"/>
-    <sheet name="Controle de Estoque" sheetId="51" state="hidden" r:id="rId3"/>
-    <sheet name="Controle de EstoqueDELET" sheetId="49" state="hidden" r:id="rId4"/>
-    <sheet name="Base de Dados2" sheetId="47" state="hidden" r:id="rId5"/>
-    <sheet name="Gerentes" sheetId="48" state="hidden" r:id="rId6"/>
-    <sheet name="." sheetId="44" state="hidden" r:id="rId7"/>
+    <sheet name="Análise" sheetId="56" r:id="rId1"/>
+    <sheet name="Base de Dados" sheetId="33" r:id="rId2"/>
+    <sheet name="Formatação" sheetId="55" state="hidden" r:id="rId3"/>
+    <sheet name="Controle de Estoque" sheetId="51" state="hidden" r:id="rId4"/>
+    <sheet name="Controle de EstoqueDELET" sheetId="49" state="hidden" r:id="rId5"/>
+    <sheet name="Base de Dados2" sheetId="47" state="hidden" r:id="rId6"/>
+    <sheet name="Gerentes" sheetId="48" state="hidden" r:id="rId7"/>
+    <sheet name="." sheetId="44" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Base de Dados2'!$A$1:$I$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Controle de Estoque'!$E$1:$F$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Base de Dados2'!$A$1:$I$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Controle de Estoque'!$E$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId9"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="108">
   <si>
     <t>Carlos Eduardo</t>
   </si>
@@ -358,6 +362,18 @@
   </si>
   <si>
     <t>Entre R$ 100,00 a R$ 500,00</t>
+  </si>
+  <si>
+    <t>Rótulos de Linha</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>Soma de Quantidade</t>
+  </si>
+  <si>
+    <t>(Tudo)</t>
   </si>
 </sst>
 </file>
@@ -658,7 +674,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -751,136 +767,14 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -943,6 +837,24 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1045,6 +957,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1061,11 +980,110 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="medium">
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </bottom>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1296,18 +1314,630 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Victor Amato dos Santos Filho" refreshedDate="45979.36256076389" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="34" xr:uid="{248E10CE-BA8F-43BF-BBA4-729ACDB95656}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabela5"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="ID" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="34"/>
+    </cacheField>
+    <cacheField name="Data da Compra" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2015-03-18T00:00:00" maxDate="2020-10-11T00:00:00"/>
+    </cacheField>
+    <cacheField name="Produto" numFmtId="0">
+      <sharedItems count="27">
+        <s v="Lancheira Básica"/>
+        <s v="Lancheira Premium Completa"/>
+        <s v="Caderno Pautado 150 Fl Pq"/>
+        <s v="Mouse Básico"/>
+        <s v="Camisa Branca P"/>
+        <s v="Teclado Wireless"/>
+        <s v="Giz de cera Pequeno 12 Cores"/>
+        <s v="Caneta 4 Cores P5"/>
+        <s v="Fichário"/>
+        <s v="Pistola de cola quente"/>
+        <s v="Esquadro Color"/>
+        <s v="Estojo Modelo Pano"/>
+        <s v="Short Preto G"/>
+        <s v="Camisa Branca M"/>
+        <s v="Avental"/>
+        <s v="Giz de cera Grande 24 Cores"/>
+        <s v="Resma Papel A4"/>
+        <s v="Borracha Branca Protector P20"/>
+        <s v="Caneta Azul P10"/>
+        <s v="Caderno Pautado 300 Fl"/>
+        <s v="Esquadro Transparente"/>
+        <s v="Projetor 720"/>
+        <s v="Cola Bastão"/>
+        <s v="Tinta Aquarela Azul"/>
+        <s v="Cola 500 ml"/>
+        <s v="Tesoura Premium"/>
+        <s v="PenDrive 128 Gb"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Preço" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="12.52" maxValue="458.32"/>
+    </cacheField>
+    <cacheField name="Vendedor" numFmtId="0">
+      <sharedItems count="32">
+        <s v="Ana Beatriz Trindade"/>
+        <s v="Israel Becker"/>
+        <s v="Cecília Tavares"/>
+        <s v="Yuri Xavier"/>
+        <s v="Pietra Lopes"/>
+        <s v="Fernanda Neves"/>
+        <s v="André Lopes"/>
+        <s v="Vitória Siqueira"/>
+        <s v="Daniel Nascimento"/>
+        <s v="Maria Fernanda Carvalho"/>
+        <s v="Pietro Nascimento"/>
+        <s v="Ana Laura Noronha"/>
+        <s v="Luna Nascimento Sampaio"/>
+        <s v="Pedro Lucas Frota"/>
+        <s v="Davi Uchoa"/>
+        <s v="Davi Miguel Neves"/>
+        <s v="Thomas Junqueira"/>
+        <s v="Maria Isis Trindade"/>
+        <s v="Yago Frota"/>
+        <s v="Gael Xavier"/>
+        <s v="Carlos Eduardo"/>
+        <s v="Arthur Henrique Pires"/>
+        <s v="Lorenzo Rangel"/>
+        <s v="Guilherme Valença"/>
+        <s v="Letícia Peçanha"/>
+        <s v="Pietro Lopes"/>
+        <s v="Lucas Barros"/>
+        <s v="Catarina Penteado"/>
+        <s v="Arthur Miguel dos Santos"/>
+        <s v="Erick Frota"/>
+        <s v="Arthur Pereira"/>
+        <s v="Emilly Pimenta"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sexo" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Feminino"/>
+        <s v="Masculino"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Quantidade" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="15" count="9">
+        <n v="7"/>
+        <n v="9"/>
+        <n v="5"/>
+        <n v="8"/>
+        <n v="14"/>
+        <n v="11"/>
+        <n v="15"/>
+        <n v="10"/>
+        <n v="13"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Forma de Pagamento" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Loja" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Santa Catarina"/>
+        <s v="São Paulo"/>
+        <s v="Rio de Janeiro"/>
+        <s v="Rio Grande do Sul"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="34">
+  <r>
+    <n v="1"/>
+    <d v="2017-09-02T00:00:00"/>
+    <x v="0"/>
+    <n v="43.36"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Cartão de Crédito"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <d v="2016-06-14T00:00:00"/>
+    <x v="1"/>
+    <n v="45.36"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Transferência Bancária"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <d v="2020-04-25T00:00:00"/>
+    <x v="2"/>
+    <n v="12.52"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="Cartão de Crédito"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <d v="2015-07-15T00:00:00"/>
+    <x v="3"/>
+    <n v="25.87"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <d v="2020-01-06T00:00:00"/>
+    <x v="4"/>
+    <n v="18.559999999999999"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="Boleto"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <d v="2015-03-18T00:00:00"/>
+    <x v="5"/>
+    <n v="202.47"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <d v="2020-03-06T00:00:00"/>
+    <x v="6"/>
+    <n v="13.25"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Transferência Bancária"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <d v="2018-02-10T00:00:00"/>
+    <x v="7"/>
+    <n v="18.96"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <d v="2018-12-07T00:00:00"/>
+    <x v="8"/>
+    <n v="17.98"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Boleto"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <d v="2020-03-11T00:00:00"/>
+    <x v="9"/>
+    <n v="18.98"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="Transferência Bancária"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <d v="2018-07-26T00:00:00"/>
+    <x v="10"/>
+    <n v="13.85"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <d v="2018-10-19T00:00:00"/>
+    <x v="11"/>
+    <n v="25.98"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="Cartão de Crédito"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <d v="2019-08-09T00:00:00"/>
+    <x v="12"/>
+    <n v="18.98"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Boleto"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <d v="2018-02-16T00:00:00"/>
+    <x v="13"/>
+    <n v="18.559999999999999"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="6"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <d v="2020-10-10T00:00:00"/>
+    <x v="14"/>
+    <n v="13.36"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Cartão de Crédito"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <d v="2020-09-30T00:00:00"/>
+    <x v="15"/>
+    <n v="29.98"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Cartão de Crédito"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <d v="2015-09-10T00:00:00"/>
+    <x v="5"/>
+    <n v="202.47"/>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <d v="2016-02-27T00:00:00"/>
+    <x v="16"/>
+    <n v="35.619999999999997"/>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="7"/>
+    <s v="Transferência Bancária"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <d v="2016-06-15T00:00:00"/>
+    <x v="17"/>
+    <n v="33.99"/>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <d v="2016-01-20T00:00:00"/>
+    <x v="18"/>
+    <n v="17.2"/>
+    <x v="17"/>
+    <x v="0"/>
+    <x v="6"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <d v="2018-04-05T00:00:00"/>
+    <x v="19"/>
+    <n v="28.9"/>
+    <x v="18"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Boleto"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <d v="2018-03-15T00:00:00"/>
+    <x v="0"/>
+    <n v="43.36"/>
+    <x v="19"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <d v="2015-07-04T00:00:00"/>
+    <x v="5"/>
+    <n v="202.47"/>
+    <x v="20"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Transferência Bancária"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <d v="2016-05-01T00:00:00"/>
+    <x v="8"/>
+    <n v="17.98"/>
+    <x v="21"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Cartão de Crédito"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <d v="2017-04-29T00:00:00"/>
+    <x v="20"/>
+    <n v="13.65"/>
+    <x v="22"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <d v="2018-01-07T00:00:00"/>
+    <x v="21"/>
+    <n v="458.32"/>
+    <x v="23"/>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Cartão de Crédito"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <d v="2015-05-21T00:00:00"/>
+    <x v="5"/>
+    <n v="202.47"/>
+    <x v="24"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <d v="2020-03-17T00:00:00"/>
+    <x v="22"/>
+    <n v="13.89"/>
+    <x v="25"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <d v="2015-08-30T00:00:00"/>
+    <x v="5"/>
+    <n v="202.47"/>
+    <x v="26"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Transferência Bancária"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <d v="2019-05-23T00:00:00"/>
+    <x v="23"/>
+    <n v="30.98"/>
+    <x v="27"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="Boleto"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <d v="2018-03-13T00:00:00"/>
+    <x v="24"/>
+    <n v="16.95"/>
+    <x v="28"/>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Cartão de Crédito"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <d v="2019-07-03T00:00:00"/>
+    <x v="25"/>
+    <n v="26.85"/>
+    <x v="29"/>
+    <x v="1"/>
+    <x v="8"/>
+    <s v="Transferência Bancária"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <d v="2016-03-06T00:00:00"/>
+    <x v="24"/>
+    <n v="16.95"/>
+    <x v="30"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Boleto"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <d v="2018-06-22T00:00:00"/>
+    <x v="26"/>
+    <n v="65"/>
+    <x v="31"/>
+    <x v="0"/>
+    <x v="6"/>
+    <s v="Transferência Bancária"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{23EA6F8F-A79D-445F-BA6E-E6DB6F550451}" name="Tabela dinâmica1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="33">
+        <item x="0"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="21"/>
+        <item x="28"/>
+        <item x="30"/>
+        <item x="20"/>
+        <item x="27"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="14"/>
+        <item x="31"/>
+        <item x="29"/>
+        <item x="5"/>
+        <item x="19"/>
+        <item x="23"/>
+        <item x="1"/>
+        <item x="24"/>
+        <item x="22"/>
+        <item x="26"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="25"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="7"/>
+        <item x="18"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="10">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="8" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Soma de Quantidade" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F85FD26-556B-43AB-B928-BB7EDDEA45C8}" name="Tabela5" displayName="Tabela5" ref="A1:I35" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F85FD26-556B-43AB-B928-BB7EDDEA45C8}" name="Tabela5" displayName="Tabela5" ref="A1:I35" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9D5B3798-EB9C-44C2-9C07-D909EA7BE2F4}" name="ID" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{C72BCE22-E506-4687-9EDB-55B1EC8C31E6}" name="Data da Compra" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{F9780277-382A-4819-9B2B-C96C10372FFC}" name="Produto" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{C1B5C037-6074-40FC-9DC6-6CDB3C382867}" name="Preço" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{1B9ECE17-3D14-431E-B8C1-5BD0BDFFE97A}" name="Vendedor" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{EEBECF56-3149-4E45-BDAF-2F9A2AD4AF3F}" name="Sexo" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{CE1B46D3-E02E-4E47-9583-730028344119}" name="Quantidade" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{7E903ED6-0492-49C0-857C-980A35CC4F2B}" name="Forma de Pagamento" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{08736880-1711-4F95-B000-B1D45644BE6A}" name="Loja" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{9D5B3798-EB9C-44C2-9C07-D909EA7BE2F4}" name="ID" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{C72BCE22-E506-4687-9EDB-55B1EC8C31E6}" name="Data da Compra" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{F9780277-382A-4819-9B2B-C96C10372FFC}" name="Produto" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C1B5C037-6074-40FC-9DC6-6CDB3C382867}" name="Preço" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{1B9ECE17-3D14-431E-B8C1-5BD0BDFFE97A}" name="Vendedor" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EEBECF56-3149-4E45-BDAF-2F9A2AD4AF3F}" name="Sexo" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{CE1B46D3-E02E-4E47-9583-730028344119}" name="Quantidade" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{7E903ED6-0492-49C0-857C-980A35CC4F2B}" name="Forma de Pagamento" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{08736880-1711-4F95-B000-B1D45644BE6A}" name="Loja" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1321,15 +1951,15 @@
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E894610B-B4D8-4C31-BF19-83D2B8A3DF15}" name="ID"/>
-    <tableColumn id="10" xr3:uid="{5313CABC-7B44-42D0-AF6B-7971EDADB5CF}" name="Data da Venda" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{06EA4EE2-DD4B-4A7B-B5A5-C4C628E8EFAE}" name="Produto" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{5E9C2846-B262-431B-B433-87EDF226E18D}" name="Preço" dataDxfId="16" dataCellStyle="Moeda"/>
-    <tableColumn id="5" xr3:uid="{D38BDC12-771F-431D-AE02-01EA9FD71B35}" name="Vendedor" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{C94DC7C2-A001-49BB-B00B-979DA1ADE426}" name="Sexo" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{31DA6D32-D514-4AC2-A931-E0B531605262}" name="Quantidade" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{3125BF66-1FFE-4D8C-9A27-7B89954726BF}" name="Forma de Pagamento" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{494CDBB5-DEE6-49AB-91BA-4632DEAE312E}" name="Loja" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{F2CC4DFF-0855-4BB4-932D-9199EBD86716}" name="Faturamento Total" dataDxfId="10">
+    <tableColumn id="10" xr3:uid="{5313CABC-7B44-42D0-AF6B-7971EDADB5CF}" name="Data da Venda" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{06EA4EE2-DD4B-4A7B-B5A5-C4C628E8EFAE}" name="Produto" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{5E9C2846-B262-431B-B433-87EDF226E18D}" name="Preço" dataDxfId="27" dataCellStyle="Moeda"/>
+    <tableColumn id="5" xr3:uid="{D38BDC12-771F-431D-AE02-01EA9FD71B35}" name="Vendedor" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{C94DC7C2-A001-49BB-B00B-979DA1ADE426}" name="Sexo" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{31DA6D32-D514-4AC2-A931-E0B531605262}" name="Quantidade" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{3125BF66-1FFE-4D8C-9A27-7B89954726BF}" name="Forma de Pagamento" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{494CDBB5-DEE6-49AB-91BA-4632DEAE312E}" name="Loja" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{F2CC4DFF-0855-4BB4-932D-9199EBD86716}" name="Faturamento Total" dataDxfId="21">
       <calculatedColumnFormula>PRODUCT(Tabela54[[#This Row],[Preço]],Tabela54[[#This Row],[Quantidade]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1338,20 +1968,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D4AD4DDD-2574-49C1-A3DE-83F8B17E2E15}" name="Tabela49" displayName="Tabela49" ref="A1:F28" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D4AD4DDD-2574-49C1-A3DE-83F8B17E2E15}" name="Tabela49" displayName="Tabela49" ref="A1:F28" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:F28" xr:uid="{D4AD4DDD-2574-49C1-A3DE-83F8B17E2E15}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
     <sortCondition ref="A1:A28"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{76E77B95-4E89-4625-A729-F9CDB9852962}" name="Produto"/>
-    <tableColumn id="2" xr3:uid="{D64EF3A7-D610-45D3-9A0E-5BA8536541EF}" name="Preço" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{94FFF367-43A3-4C6E-9594-51FF526D144B}" name="Entradas" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{C7711B3E-0857-4032-AD68-7E5B107E9850}" name="Saídas" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{0806FA7A-E31D-4D0B-A528-FD9D983CAA77}" name="Estoque final" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{D64EF3A7-D610-45D3-9A0E-5BA8536541EF}" name="Preço" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{94FFF367-43A3-4C6E-9594-51FF526D144B}" name="Entradas" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{C7711B3E-0857-4032-AD68-7E5B107E9850}" name="Saídas" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{0806FA7A-E31D-4D0B-A528-FD9D983CAA77}" name="Estoque final" dataDxfId="16">
       <calculatedColumnFormula>Tabela49[[#This Row],[Entradas]]-Tabela49[[#This Row],[Saídas]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{D2CFE065-FACB-4CF1-B660-0AD821CF9983}" name="Faturamento total" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{D2CFE065-FACB-4CF1-B660-0AD821CF9983}" name="Faturamento total" dataDxfId="15">
       <calculatedColumnFormula>PRODUCT(Tabela49[[#This Row],[Preço]],Tabela49[[#This Row],[Saídas]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1360,7 +1990,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8602B678-8888-4FFF-910E-E37E8488DFDD}" name="Tabela4" displayName="Tabela4" ref="A1:D28" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8602B678-8888-4FFF-910E-E37E8488DFDD}" name="Tabela4" displayName="Tabela4" ref="A1:D28" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:D28" xr:uid="{8602B678-8888-4FFF-910E-E37E8488DFDD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D28">
     <sortCondition ref="A1:A28"/>
@@ -1369,7 +1999,7 @@
     <tableColumn id="1" xr3:uid="{F6B38D27-FFAE-4128-A147-9D5850FF36D0}" name="Produto"/>
     <tableColumn id="2" xr3:uid="{BB73B33A-F392-4B5C-8768-271AED9517EB}" name="Preço"/>
     <tableColumn id="5" xr3:uid="{A75FD632-D648-4FC4-AE4F-D12C23355447}" name="Entradas"/>
-    <tableColumn id="6" xr3:uid="{B2603A0C-E740-42F5-973F-EF9D1C1E2F45}" name="Saídas" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{B2603A0C-E740-42F5-973F-EF9D1C1E2F45}" name="Saídas" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1671,11 +2301,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6F7565-2EE9-4D2D-89AF-84F056CEEFB0}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="32" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="49">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="49">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="49">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9D9A69-828D-46F6-A798-5EB77C96CE73}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2722,7 +3414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{954A7C27-229D-4ADD-ADA5-EE274BACF150}">
   <dimension ref="A1:M35"/>
   <sheetViews>
@@ -3935,7 +4627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBC40A6-82FC-4108-9442-D5E8FCC459E6}">
   <dimension ref="A1:K28"/>
   <sheetViews>
@@ -4608,7 +5300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC509290-CF3F-4CB7-AF42-5C43800EFADB}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -4957,7 +5649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3863EAD-412C-42D6-A81B-8FF3AEF54D5F}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -6004,7 +6696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5E284B-E125-4EA7-B323-858B33C92270}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -6088,7 +6780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF49DD56-C9C3-4138-AEEC-5247B0334F0B}">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>